<commit_message>
label ms on it
</commit_message>
<xml_diff>
--- a/PA1/doc/compare.xlsx
+++ b/PA1/doc/compare.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Shannon/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Shannon/Documents/AlgorithMew/PA1/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4B90B6F-3FCF-BA44-AAD0-76B7E8702E1C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AFEB5CC-EC28-D44D-B28C-65838D1E944B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3980" yWindow="460" windowWidth="21700" windowHeight="15000" xr2:uid="{45BA81B1-19C9-C345-92CA-5FDA527F255E}"/>
+    <workbookView xWindow="3900" yWindow="460" windowWidth="21700" windowHeight="15000" xr2:uid="{45BA81B1-19C9-C345-92CA-5FDA527F255E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -40,9 +40,6 @@
   </si>
   <si>
     <t>HS</t>
-  </si>
-  <si>
-    <t>CPU time(s)</t>
   </si>
   <si>
     <t>Memory(KB)</t>
@@ -103,6 +100,9 @@
   </si>
   <si>
     <t>case3</t>
+  </si>
+  <si>
+    <t>CPU time(ms)</t>
   </si>
 </sst>
 </file>
@@ -174,11 +174,11 @@
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -233,6 +233,15 @@
               <a:rPr lang="en-US"/>
               <a:t>case1</a:t>
             </a:r>
+            <a:r>
+              <a:rPr lang="zh-TW" altLang="en-US"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-TW"/>
+              <a:t>(ms-inputsize)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -810,6 +819,15 @@
               <a:rPr lang="en-US"/>
               <a:t>case2</a:t>
             </a:r>
+            <a:r>
+              <a:rPr lang="zh-TW" altLang="en-US"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-TW"/>
+              <a:t>(ms-inputsize)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -1385,8 +1403,19 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>case3</a:t>
+              <a:t>case3 </a:t>
             </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>(ms-inputsize)</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -1962,7 +1991,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>case1</a:t>
+              <a:t>case1 (ms-inputsize)</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -2540,8 +2569,19 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>case2</a:t>
+              <a:t>case2 </a:t>
             </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>(ms-inputsize)</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -3118,8 +3158,19 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>case3</a:t>
+              <a:t>case3 </a:t>
             </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>(ms-inputsize)</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -7527,83 +7578,87 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEAE15E8-25EF-3540-8F2E-350AADAF779D}">
   <dimension ref="A2:P21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C20" zoomScale="85" zoomScaleNormal="82" workbookViewId="0">
-      <selection activeCell="Q54" sqref="Q54"/>
+    <sheetView tabSelected="1" zoomScale="89" zoomScaleNormal="82" workbookViewId="0">
+      <selection activeCell="W35" sqref="W35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="14.83203125" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" customWidth="1"/>
+    <col min="7" max="7" width="11.83203125" customWidth="1"/>
+    <col min="9" max="9" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="L2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
-      <c r="O2" s="2"/>
-      <c r="P2" s="2"/>
+      <c r="L2" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
+      <c r="O2" s="4"/>
+      <c r="P2" s="4"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2" t="s">
+      <c r="D3" s="4"/>
+      <c r="E3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2" t="s">
+      <c r="F3" s="4"/>
+      <c r="G3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2" t="s">
+      <c r="H3" s="4"/>
+      <c r="I3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="J3" s="2"/>
+      <c r="J3" s="4"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N3" s="1" t="s">
+      <c r="O3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="O3" s="1" t="s">
+      <c r="P3" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>6</v>
-      </c>
       <c r="E4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>6</v>
-      </c>
       <c r="G4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="1" t="s">
-        <v>6</v>
-      </c>
       <c r="I4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J4" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>6</v>
       </c>
       <c r="L4" s="1">
         <v>4000</v>
@@ -7626,7 +7681,7 @@
         <v>4000</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5" s="1">
         <v>0</v>
@@ -7673,7 +7728,7 @@
         <v>4000</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C6" s="1">
         <v>4</v>
@@ -7720,7 +7775,7 @@
         <v>4000</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C7" s="1">
         <v>0</v>
@@ -7767,7 +7822,7 @@
         <v>16000</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C8" s="1">
         <v>0</v>
@@ -7799,7 +7854,7 @@
         <v>16000</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C9" s="1">
         <v>68</v>
@@ -7825,20 +7880,20 @@
       <c r="J9" s="1">
         <v>13428</v>
       </c>
-      <c r="L9" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="M9" s="2"/>
-      <c r="N9" s="2"/>
-      <c r="O9" s="2"/>
-      <c r="P9" s="2"/>
+      <c r="L9" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="M9" s="4"/>
+      <c r="N9" s="4"/>
+      <c r="O9" s="4"/>
+      <c r="P9" s="4"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>16000</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>10</v>
+      <c r="B10" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="C10" s="1">
         <v>32</v>
@@ -7866,16 +7921,16 @@
       </c>
       <c r="L10" s="1"/>
       <c r="M10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N10" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N10" s="1" t="s">
+      <c r="O10" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="O10" s="1" t="s">
+      <c r="P10" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="P10" s="1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
@@ -7883,7 +7938,7 @@
         <v>32000</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C11" s="1">
         <v>0</v>
@@ -7930,7 +7985,7 @@
         <v>32000</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C12" s="1">
         <v>260</v>
@@ -7977,7 +8032,7 @@
         <v>32000</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C13" s="1">
         <v>128</v>
@@ -8006,16 +8061,16 @@
       <c r="L13" s="1">
         <v>32000</v>
       </c>
-      <c r="M13" s="4">
+      <c r="M13" s="3">
         <v>0</v>
       </c>
-      <c r="N13" s="4">
+      <c r="N13" s="3">
         <v>0</v>
       </c>
-      <c r="O13" s="4">
+      <c r="O13" s="3">
         <v>308</v>
       </c>
-      <c r="P13" s="4">
+      <c r="P13" s="3">
         <v>0</v>
       </c>
     </row>
@@ -8024,7 +8079,7 @@
         <v>1000000</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C14" s="1">
         <v>0</v>
@@ -8071,7 +8126,7 @@
         <v>1000000</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C15" s="1">
         <v>244412</v>
@@ -8103,7 +8158,7 @@
         <v>1000000</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C16" s="1">
         <v>123392</v>
@@ -8129,27 +8184,27 @@
       <c r="J16" s="1">
         <v>19452</v>
       </c>
-      <c r="L16" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="M16" s="2"/>
-      <c r="N16" s="2"/>
-      <c r="O16" s="2"/>
-      <c r="P16" s="2"/>
+      <c r="L16" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="M16" s="4"/>
+      <c r="N16" s="4"/>
+      <c r="O16" s="4"/>
+      <c r="P16" s="4"/>
     </row>
     <row r="17" spans="12:16" x14ac:dyDescent="0.2">
       <c r="L17" s="1"/>
       <c r="M17" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N17" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N17" s="1" t="s">
+      <c r="O17" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="O17" s="1" t="s">
+      <c r="P17" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="P17" s="1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="18" spans="12:16" x14ac:dyDescent="0.2">
@@ -8222,13 +8277,13 @@
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="L2:P2"/>
+    <mergeCell ref="L9:P9"/>
     <mergeCell ref="L16:P16"/>
     <mergeCell ref="I3:J3"/>
     <mergeCell ref="G3:H3"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="C3:D3"/>
-    <mergeCell ref="L2:P2"/>
-    <mergeCell ref="L9:P9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>